<commit_message>
medicion carril derecho ciclovia
se inicio la medicion del carril derecho de la ciclo via
</commit_message>
<xml_diff>
--- a/Copia de Formulario_Plantilla_BasicaSenalizacion_v2_11_2016_Ciclorruta Las Vegas (002).xlsx
+++ b/Copia de Formulario_Plantilla_BasicaSenalizacion_v2_11_2016_Ciclorruta Las Vegas (002).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JUAN_PC\Documents\GitHub\cicloruta\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27EE6A78-4608-4258-BC15-4826B92DF4CA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46AFE062-BB95-44F7-B273-6F4679FD2D45}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9450" tabRatio="711" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2333,7 +2333,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3928" uniqueCount="855">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3929" uniqueCount="856">
   <si>
     <t>ID_OP</t>
   </si>
@@ -4898,6 +4898,9 @@
   </si>
   <si>
     <t>tach´s</t>
+  </si>
+  <si>
+    <t>dist</t>
   </si>
 </sst>
 </file>
@@ -5392,7 +5395,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="41" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="181">
+  <cellXfs count="182">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
@@ -5738,6 +5741,7 @@
     <xf numFmtId="3" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="1" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="7" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="1" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Millares [0]" xfId="4" builtinId="6"/>
@@ -6085,8 +6089,8 @@
   </sheetPr>
   <dimension ref="A1:R1006"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D390" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G407" sqref="G407"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F120" sqref="F120:G120"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.3"/>
@@ -6102,12 +6106,12 @@
     <col min="9" max="9" width="18.7109375" style="123" customWidth="1"/>
     <col min="10" max="10" width="12.7109375" style="123" customWidth="1"/>
     <col min="11" max="11" width="12.42578125" style="123" customWidth="1"/>
-    <col min="12" max="12" width="17.28515625" style="123" customWidth="1"/>
-    <col min="13" max="13" width="17.5703125" style="123" customWidth="1"/>
-    <col min="14" max="14" width="13.28515625" style="130" customWidth="1"/>
-    <col min="15" max="15" width="17.7109375" style="130" customWidth="1"/>
+    <col min="12" max="12" width="12.85546875" style="123" customWidth="1"/>
+    <col min="13" max="13" width="11.140625" style="123" customWidth="1"/>
+    <col min="14" max="14" width="9.28515625" style="130" customWidth="1"/>
+    <col min="15" max="15" width="10.42578125" style="130" customWidth="1"/>
     <col min="16" max="16" width="10.42578125" style="123" customWidth="1"/>
-    <col min="17" max="17" width="37" style="123" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="10" style="123" customWidth="1"/>
     <col min="18" max="18" width="55" style="123" bestFit="1" customWidth="1"/>
     <col min="19" max="16384" width="11.42578125" style="123"/>
   </cols>
@@ -9972,8 +9976,12 @@
       <c r="E119" s="2">
         <v>1</v>
       </c>
-      <c r="F119" s="132"/>
-      <c r="G119" s="132"/>
+      <c r="F119" s="161">
+        <v>180260</v>
+      </c>
+      <c r="G119" s="161">
+        <v>180260</v>
+      </c>
       <c r="I119" s="2" t="s">
         <v>73</v>
       </c>
@@ -10001,8 +10009,12 @@
       <c r="E120" s="2">
         <v>1</v>
       </c>
-      <c r="F120" s="132"/>
-      <c r="G120" s="132"/>
+      <c r="F120" s="161">
+        <v>180260</v>
+      </c>
+      <c r="G120" s="161">
+        <v>180260</v>
+      </c>
       <c r="I120" s="2" t="s">
         <v>73</v>
       </c>
@@ -11116,35 +11128,35 @@
         <v>838</v>
       </c>
     </row>
-    <row r="164" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A164" s="104">
+    <row r="164" spans="1:18" s="169" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A164" s="147">
         <v>2000029</v>
       </c>
-      <c r="B164" s="2">
+      <c r="B164" s="169">
         <v>2</v>
       </c>
-      <c r="C164" s="2">
+      <c r="C164" s="169">
         <v>2</v>
       </c>
-      <c r="E164" s="2">
+      <c r="E164" s="169">
         <v>-1</v>
       </c>
-      <c r="F164" s="132"/>
-      <c r="G164" s="132"/>
-      <c r="I164" s="31" t="s">
+      <c r="F164" s="136"/>
+      <c r="G164" s="136"/>
+      <c r="I164" s="180" t="s">
         <v>92</v>
       </c>
-      <c r="J164" s="62" t="s">
+      <c r="J164" s="170" t="s">
         <v>8</v>
       </c>
-      <c r="K164" s="15" t="s">
+      <c r="K164" s="175" t="s">
         <v>6</v>
       </c>
-      <c r="P164" s="17"/>
-      <c r="Q164" t="s">
+      <c r="P164" s="171"/>
+      <c r="Q164" s="172" t="s">
         <v>768</v>
       </c>
-      <c r="R164" s="32" t="s">
+      <c r="R164" s="173" t="s">
         <v>93</v>
       </c>
     </row>
@@ -12155,7 +12167,7 @@
         <v>112708</v>
       </c>
       <c r="G196" s="168">
-        <f t="shared" ref="G196:G214" si="7">F196-504</f>
+        <f t="shared" ref="G196:G213" si="7">F196-504</f>
         <v>112204</v>
       </c>
       <c r="K196" s="62" t="s">
@@ -14305,65 +14317,65 @@
         <v>837</v>
       </c>
     </row>
-    <row r="267" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A267" s="104">
+    <row r="267" spans="1:18" s="169" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A267" s="147">
         <v>2000029</v>
       </c>
-      <c r="B267" s="2">
+      <c r="B267" s="169">
         <v>4</v>
       </c>
-      <c r="C267" s="2">
+      <c r="C267" s="169">
         <v>2</v>
       </c>
-      <c r="E267" s="2">
-        <v>1</v>
-      </c>
-      <c r="F267" s="132"/>
-      <c r="G267" s="132"/>
-      <c r="I267" s="31" t="s">
+      <c r="E267" s="169">
+        <v>1</v>
+      </c>
+      <c r="F267" s="136"/>
+      <c r="G267" s="136"/>
+      <c r="I267" s="180" t="s">
         <v>92</v>
       </c>
-      <c r="J267" s="62" t="s">
+      <c r="J267" s="170" t="s">
         <v>8</v>
       </c>
-      <c r="K267" s="15" t="s">
+      <c r="K267" s="175" t="s">
         <v>6</v>
       </c>
-      <c r="P267" s="17"/>
-      <c r="Q267" t="s">
+      <c r="P267" s="171"/>
+      <c r="Q267" s="172" t="s">
         <v>768</v>
       </c>
-      <c r="R267" s="32" t="s">
+      <c r="R267" s="173" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="268" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A268" s="104">
+    <row r="268" spans="1:18" s="169" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A268" s="147">
         <v>2000029</v>
       </c>
-      <c r="B268" s="2">
+      <c r="B268" s="169">
         <v>2</v>
       </c>
-      <c r="C268" s="2">
+      <c r="C268" s="169">
         <v>2</v>
       </c>
-      <c r="E268" s="2">
+      <c r="E268" s="169">
         <v>-1</v>
       </c>
-      <c r="F268" s="132"/>
-      <c r="G268" s="132"/>
-      <c r="I268" s="15"/>
-      <c r="J268" s="15" t="s">
+      <c r="F268" s="136"/>
+      <c r="G268" s="136"/>
+      <c r="I268" s="175"/>
+      <c r="J268" s="175" t="s">
         <v>8</v>
       </c>
-      <c r="K268" s="15" t="s">
+      <c r="K268" s="175" t="s">
         <v>7</v>
       </c>
-      <c r="P268" s="17"/>
-      <c r="Q268" t="s">
+      <c r="P268" s="171"/>
+      <c r="Q268" s="172" t="s">
         <v>768</v>
       </c>
-      <c r="R268" s="113" t="s">
+      <c r="R268" s="181" t="s">
         <v>847</v>
       </c>
     </row>
@@ -14517,10 +14529,10 @@
         <v>-1</v>
       </c>
       <c r="F273" s="178">
-        <v>32260</v>
+        <v>103480</v>
       </c>
       <c r="G273" s="178">
-        <v>32260</v>
+        <v>103480</v>
       </c>
       <c r="I273" s="176"/>
       <c r="J273" s="176" t="s">
@@ -18858,7 +18870,7 @@
         <v>80430</v>
       </c>
       <c r="G407" s="174">
-        <f t="shared" si="12"/>
+        <f>F407-485</f>
         <v>79945</v>
       </c>
       <c r="K407" s="62" t="s">
@@ -19985,8 +19997,13 @@
       <c r="E450" s="2">
         <v>-1</v>
       </c>
-      <c r="F450" s="132"/>
-      <c r="G450" s="132"/>
+      <c r="F450" s="161">
+        <v>5095</v>
+      </c>
+      <c r="G450" s="161">
+        <f>F450-400</f>
+        <v>4695</v>
+      </c>
       <c r="I450" s="15" t="s">
         <v>99</v>
       </c>
@@ -20015,8 +20032,14 @@
       <c r="E451" s="2">
         <v>-1</v>
       </c>
-      <c r="F451" s="132"/>
-      <c r="G451" s="132"/>
+      <c r="F451" s="161">
+        <f>F450-400</f>
+        <v>4695</v>
+      </c>
+      <c r="G451" s="161">
+        <f t="shared" ref="G451:G454" si="14">F451-400</f>
+        <v>4295</v>
+      </c>
       <c r="I451" s="15" t="s">
         <v>99</v>
       </c>
@@ -20045,8 +20068,14 @@
       <c r="E452" s="2">
         <v>-1</v>
       </c>
-      <c r="F452" s="132"/>
-      <c r="G452" s="132"/>
+      <c r="F452" s="161">
+        <f t="shared" ref="F452:F454" si="15">F451-400</f>
+        <v>4295</v>
+      </c>
+      <c r="G452" s="161">
+        <f t="shared" si="14"/>
+        <v>3895</v>
+      </c>
       <c r="I452" s="15" t="s">
         <v>99</v>
       </c>
@@ -20075,8 +20104,14 @@
       <c r="E453" s="2">
         <v>-1</v>
       </c>
-      <c r="F453" s="132"/>
-      <c r="G453" s="132"/>
+      <c r="F453" s="161">
+        <f t="shared" si="15"/>
+        <v>3895</v>
+      </c>
+      <c r="G453" s="161">
+        <f t="shared" si="14"/>
+        <v>3495</v>
+      </c>
       <c r="I453" s="15" t="s">
         <v>99</v>
       </c>
@@ -20105,8 +20140,14 @@
       <c r="E454" s="2">
         <v>-1</v>
       </c>
-      <c r="F454" s="132"/>
-      <c r="G454" s="132"/>
+      <c r="F454" s="161">
+        <f t="shared" si="15"/>
+        <v>3495</v>
+      </c>
+      <c r="G454" s="161">
+        <f t="shared" si="14"/>
+        <v>3095</v>
+      </c>
       <c r="I454" s="15" t="s">
         <v>99</v>
       </c>
@@ -20285,7 +20326,9 @@
       <c r="E460" s="2">
         <v>-1</v>
       </c>
-      <c r="F460" s="132"/>
+      <c r="F460" s="161">
+        <v>5400</v>
+      </c>
       <c r="G460" s="132"/>
       <c r="I460" s="62" t="s">
         <v>18</v>
@@ -20296,7 +20339,9 @@
       <c r="K460" s="62" t="s">
         <v>7</v>
       </c>
-      <c r="P460" s="17"/>
+      <c r="P460" s="17" t="s">
+        <v>855</v>
+      </c>
       <c r="Q460" t="s">
         <v>768</v>
       </c>
@@ -20317,7 +20362,9 @@
       <c r="E461" s="2">
         <v>-1</v>
       </c>
-      <c r="F461" s="132"/>
+      <c r="F461" s="161">
+        <v>4780</v>
+      </c>
       <c r="G461" s="132"/>
       <c r="I461" s="15" t="s">
         <v>19</v>
@@ -20346,7 +20393,9 @@
       <c r="E462" s="2">
         <v>-1</v>
       </c>
-      <c r="F462" s="132"/>
+      <c r="F462" s="161">
+        <v>2290</v>
+      </c>
       <c r="G462" s="132"/>
       <c r="I462" s="2" t="s">
         <v>11</v>

</xml_diff>